<commit_message>
Updates NYC measles cases by neighborhood
</commit_message>
<xml_diff>
--- a/data/nyc-measles-cases-by-neighborhood.xlsx
+++ b/data/nyc-measles-cases-by-neighborhood.xlsx
@@ -8,9 +8,10 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="2019-08-19" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="2019-07-29" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="2019-07-22" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="2019-08-26" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="2019-08-19" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="2019-07-29" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="2019-07-22" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,11 +23,77 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="32">
   <si>
     <t xml:space="preserve">neighborhood</t>
   </si>
   <si>
+    <t xml:space="preserve">ongoing transmission (2019-08-26)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">all cases (2018-09-01 to 2019-08-26)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">latest cases (2019-08-19 to 2019-08-26)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Borough Park</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crown Heights</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Williamsburg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bensonhurst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brighton Beach/Coney Island</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chelsea/Clinton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Far Rockaway</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flatbush</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flushing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hunts Point/Longwood/Melrose</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jamaica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Long Island City/Astoria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Midwood/Marine Park</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Port Richmond</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Red Hook</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sunset Park</t>
+  </si>
+  <si>
+    <t xml:space="preserve">West Queens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Willowbrook</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOTAL</t>
+  </si>
+  <si>
     <t xml:space="preserve">ongoing transmission (2019-08-19)</t>
   </si>
   <si>
@@ -34,63 +101,6 @@
   </si>
   <si>
     <t xml:space="preserve">latest cases (2019-08-12 to 2019-08-19)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Borough Park</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Crown Heights</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Williamsburg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bensonhurst</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Brighton Beach/Coney Island</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chelsea/Clinton</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Far Rockaway</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flatbush</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flushing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hunts Point/Longwood/Melrose</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jamaica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Long Island City/Astoria</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Midwood/Marine Park</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Port Richmond</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Red Hook</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sunset Park</t>
-  </si>
-  <si>
-    <t xml:space="preserve">West Queens</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Willowbrook</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TOTAL</t>
   </si>
   <si>
     <t xml:space="preserve">ongoing transmission (2019-07-29)</t>
@@ -212,7 +222,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -276,7 +286,7 @@
         <v>472</v>
       </c>
       <c r="D4" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -500,7 +510,7 @@
         <v>654</v>
       </c>
       <c r="D20" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -525,6 +535,316 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="30.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="33.38"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>123</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>472</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="D14" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D15" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D16" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C17" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="D17" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D18" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C19" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="D19" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C20" s="1" t="n">
+        <v>654</v>
+      </c>
+      <c r="D20" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D20"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.32"/>
@@ -539,13 +859,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -825,7 +1145,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -850,13 +1170,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>